<commit_message>
Another update to make fonts better.
</commit_message>
<xml_diff>
--- a/Climbing Cam Load Calculator.xlsx
+++ b/Climbing Cam Load Calculator.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+  <si>
+    <t>By @Levi.io</t>
+  </si>
   <si>
     <t>Inputs</t>
   </si>
@@ -74,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -82,15 +85,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
     </font>
     <font/>
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -233,51 +240,54 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="2" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="2" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="2" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="2" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -530,152 +540,157 @@
     <col customWidth="1" min="12" max="26" width="8.63"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="3">
-      <c r="I3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="I5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="8">
+        <v>37.0</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="I6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="I7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="11">
+        <v>14.5</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9">
+      <c r="I9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="5">
-        <v>10.0</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="I5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="7">
-        <v>37.0</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="I6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="I7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="10">
-        <v>14.5</v>
-      </c>
-      <c r="K7" s="10" t="s">
+    </row>
+    <row r="10">
+      <c r="I10" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-    </row>
-    <row r="9">
-      <c r="I9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="I10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="13">
+      <c r="J10" s="14">
         <f>IF(J7&lt;&gt;"", J7, DEGREES(ATAN2(J5,J4)))</f>
         <v>14.5</v>
       </c>
-      <c r="K10" s="5"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11">
-      <c r="I11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="14">
+      <c r="I11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="15">
         <f>J6/(2*TAN(RADIANS(J10)))</f>
         <v>7.73342619</v>
       </c>
-      <c r="K11" s="9" t="s">
-        <v>12</v>
+      <c r="K11" s="10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12">
-      <c r="I12" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="16">
+      <c r="I12" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="17">
         <f>J11/J6</f>
         <v>1.933356547</v>
       </c>
-      <c r="K12" s="17" t="s">
-        <v>14</v>
+      <c r="K12" s="18" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13">
-      <c r="I13" s="18"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="16">
-      <c r="K16" s="3" t="s">
-        <v>15</v>
+      <c r="K16" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" ht="15.0" customHeight="1">
-      <c r="K17" s="20" t="s">
-        <v>16</v>
+      <c r="K17" s="21" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18">
-      <c r="K18" s="21"/>
+      <c r="K18" s="22"/>
     </row>
     <row r="19">
-      <c r="K19" s="21"/>
+      <c r="K19" s="22"/>
     </row>
     <row r="20">
-      <c r="K20" s="21"/>
+      <c r="K20" s="22"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="K21" s="21"/>
+      <c r="K21" s="22"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="K22" s="21"/>
+      <c r="K22" s="22"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="K23" s="21"/>
+      <c r="K23" s="22"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="K24" s="21"/>
+      <c r="K24" s="22"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="K25" s="21"/>
+      <c r="K25" s="22"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="K26" s="22"/>
+      <c r="K26" s="23"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="K27" s="23" t="s">
-        <v>17</v>
+      <c r="K27" s="24" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1"/>

</xml_diff>